<commit_message>
Commit final do classificador
</commit_message>
<xml_diff>
--- a/Election.xlsx
+++ b/Election.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive - Insper - Institudo de Ensino e Pesquisa\S2\CDADOS\CDADOS-P1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alinsperedu-my.sharepoint.com/personal/diegoss3_al_insper_edu_br/Documents/S2/CDADOS/CDADOS-P1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{8D793816-D3CD-4423-846A-A6D3C41F748E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{84ED21BB-F634-4D9B-B4F0-311F49B4B191}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{8D793816-D3CD-4423-846A-A6D3C41F748E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4B07EF1A-A656-4C00-B4BD-1A1C60E4B297}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2340" yWindow="2340" windowWidth="14670" windowHeight="8325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -2600,11 +2600,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="120" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -6630,7 +6633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E125"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>